<commit_message>
New Work Order Node Transfer Configuration
</commit_message>
<xml_diff>
--- a/zero-erp/src/main/resources/plugin/erp/oob/rule/process.oa.assignment/activity-rule.xlsx
+++ b/zero-erp/src/main/resources/plugin/erp/oob/rule/process.oa.assignment/activity-rule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xuanhong\zero-ws\zero-extension\zero-erp\src\main\resources\plugin\erp\oob\rule\process.oa.assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D7463E-35F6-4138-A2EE-836B23ABF982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95907B1F-A1AB-45F3-879D-3603466E1B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12624" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="123">
   <si>
     <t>key</t>
   </si>
@@ -468,6 +468,13 @@
   </si>
   <si>
     <t>df6b90dd-bbe1-4107-b2b8-26d16518ffa8</t>
+  </si>
+  <si>
+    <t>$zn.status == "DRAFT" and $zo.acceptedBy != null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9805cfa0-eb64-4772-9ba5-04814be862aa</t>
   </si>
 </sst>
 </file>
@@ -646,7 +653,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,21 +702,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1025,30 +1020,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500280C7-B0AC-7C45-9420-F2551253A777}">
-  <dimension ref="A2:P28"/>
+  <dimension ref="A2:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="111" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="92.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="52" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="92.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="81.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
@@ -1262,7 +1257,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>67</v>
@@ -1271,19 +1266,19 @@
         <v>31</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E7" s="9">
         <v>1010</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>90</v>
+        <v>47</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>34</v>
@@ -1291,7 +1286,9 @@
       <c r="J7" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="K7" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="L7" s="11" t="b">
         <v>1</v>
       </c>
@@ -1304,7 +1301,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>67</v>
@@ -1319,13 +1316,13 @@
         <v>1010</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>34</v>
@@ -1346,7 +1343,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>67</v>
@@ -1357,17 +1354,17 @@
       <c r="D9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="17">
-        <v>1015</v>
+      <c r="E9" s="9">
+        <v>1010</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>34</v>
@@ -1388,7 +1385,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>67</v>
@@ -1403,13 +1400,13 @@
         <v>1015</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>34</v>
@@ -1430,28 +1427,28 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="17">
-        <v>1005</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>37</v>
+        <v>1015</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>34</v>
@@ -1472,7 +1469,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>67</v>
@@ -1483,17 +1480,17 @@
       <c r="D12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="9">
-        <v>1010</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>95</v>
+      <c r="E12" s="17">
+        <v>1005</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>34</v>
@@ -1514,7 +1511,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>67</v>
@@ -1523,19 +1520,19 @@
         <v>36</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E13" s="9">
         <v>1010</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>87</v>
+      <c r="F13" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>34</v>
@@ -1543,9 +1540,7 @@
       <c r="J13" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K13" s="11" t="s">
-        <v>41</v>
-      </c>
+      <c r="K13" s="9"/>
       <c r="L13" s="11" t="b">
         <v>1</v>
       </c>
@@ -1558,7 +1553,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>67</v>
@@ -1567,19 +1562,19 @@
         <v>36</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E14" s="9">
-        <v>1015</v>
+        <v>1010</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>90</v>
+        <v>47</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>34</v>
@@ -1587,7 +1582,9 @@
       <c r="J14" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K14" s="9"/>
+      <c r="K14" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="L14" s="11" t="b">
         <v>1</v>
       </c>
@@ -1600,7 +1597,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>67</v>
@@ -1615,13 +1612,13 @@
         <v>1015</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>34</v>
@@ -1642,30 +1639,30 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>51</v>
       </c>
       <c r="E16" s="9">
-        <v>1005</v>
+        <v>1015</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>34</v>
       </c>
       <c r="J16" s="11" t="s">
@@ -1684,7 +1681,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>67</v>
@@ -1696,18 +1693,18 @@
         <v>51</v>
       </c>
       <c r="E17" s="9">
-        <v>1010</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>46</v>
+        <v>1005</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="18" t="s">
         <v>34</v>
       </c>
       <c r="J17" s="11" t="s">
@@ -1726,7 +1723,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>67</v>
@@ -1735,19 +1732,19 @@
         <v>44</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E18" s="9">
         <v>1010</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>47</v>
+      <c r="F18" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>34</v>
@@ -1755,9 +1752,7 @@
       <c r="J18" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>41</v>
-      </c>
+      <c r="K18" s="9"/>
       <c r="L18" s="11" t="b">
         <v>1</v>
       </c>
@@ -1770,7 +1765,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>67</v>
@@ -1779,19 +1774,19 @@
         <v>44</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E19" s="9">
-        <v>1015</v>
+        <v>1010</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I19" s="11" t="s">
         <v>34</v>
@@ -1799,7 +1794,9 @@
       <c r="J19" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K19" s="9"/>
+      <c r="K19" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="L19" s="11" t="b">
         <v>1</v>
       </c>
@@ -1812,7 +1809,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>67</v>
@@ -1827,13 +1824,13 @@
         <v>1015</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>34</v>
@@ -1854,7 +1851,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>67</v>
@@ -1866,18 +1863,18 @@
         <v>51</v>
       </c>
       <c r="E21" s="9">
-        <v>1020</v>
+        <v>1015</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="I21" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>34</v>
       </c>
       <c r="J21" s="11" t="s">
@@ -1895,318 +1892,360 @@
       <c r="P21" s="11"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1020</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" s="11"/>
+      <c r="N22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="26" t="s">
+      <c r="B23" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D23" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E23" s="9">
         <v>2005</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F23" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G23" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H23" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="I22" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J22" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="K22" s="27" t="s">
+      <c r="I23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K23" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="L22" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M22" s="27"/>
-      <c r="N22" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
+      <c r="L23" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" s="11"/>
+      <c r="N23" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="26" t="s">
+      <c r="B24" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D24" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E24" s="9">
         <v>2005</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F24" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G24" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H24" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="I23" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="K23" s="27" t="s">
+      <c r="I24" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K24" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="L23" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M23" s="27"/>
-      <c r="N23" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A24" s="24" t="s">
+      <c r="L24" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" s="11"/>
+      <c r="N24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="26" t="s">
+      <c r="B25" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D25" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E25" s="9">
         <v>2005</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F25" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G25" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H25" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="I24" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="K24" s="27" t="s">
+      <c r="I25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K25" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="L24" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M24" s="27"/>
-      <c r="N24" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A25" s="24" t="s">
+      <c r="L25" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" s="11"/>
+      <c r="N25" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="26" t="s">
+      <c r="B26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D26" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E26" s="9">
         <v>2005</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F26" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G26" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H26" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="K25" s="27" t="s">
+      <c r="I26" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K26" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="L25" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M25" s="27"/>
-      <c r="N25" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A26" s="24" t="s">
+      <c r="L26" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" s="11"/>
+      <c r="N26" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="26" t="s">
+      <c r="B27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D27" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E27" s="9">
         <v>2010</v>
       </c>
-      <c r="F26" s="27" t="s">
+      <c r="F27" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="30" t="s">
+      <c r="G27" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H26" s="27" t="s">
+      <c r="H27" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="I26" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="K26" s="27" t="s">
+      <c r="I27" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K27" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="L26" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M26" s="27" t="s">
+      <c r="L27" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="N26" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A27" s="24" t="s">
+      <c r="N27" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="26" t="s">
+      <c r="B28" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D28" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E28" s="9">
         <v>2010</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F28" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G28" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H27" s="27" t="s">
+      <c r="H28" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="I27" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="K27" s="27" t="s">
+      <c r="I28" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K28" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="L27" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M27" s="27" t="s">
+      <c r="L28" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="N27" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A28" s="24" t="s">
+      <c r="N28" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="26" t="s">
+      <c r="B29" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D29" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E29" s="9">
         <v>2010</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F29" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G29" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H28" s="27" t="s">
+      <c r="H29" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="I28" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J28" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="K28" s="27" t="s">
+      <c r="I29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K29" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="L28" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M28" s="27" t="s">
+      <c r="L29" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M29" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="N28" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
+      <c r="N29" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>